<commit_message>
excel file reading func
</commit_message>
<xml_diff>
--- a/test_price.xlsx
+++ b/test_price.xlsx
@@ -3,59 +3,44 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="18080" windowWidth="15960" xWindow="0" yWindow="40"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>transaction_id</t>
-  </si>
-  <si>
-    <t>product_id</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
+      <name val="Helvetica Neue"/>
+      <color indexed="8"/>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
+      <name val="Helvetica Neue"/>
+      <color indexed="8"/>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
+      <name val="Helvetica Neue"/>
+      <color indexed="8"/>
       <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
+      <name val="Helvetica Neue"/>
       <b val="1"/>
+      <color indexed="8"/>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -173,59 +158,126 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="9">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="3" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf applyAlignment="1" borderId="2" fillId="3" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf applyAlignment="1" borderId="3" fillId="3" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf applyAlignment="1" borderId="4" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf applyAlignment="1" borderId="5" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf applyAlignment="1" borderId="6" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet 1'!$D$2:$D$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1285,89 +1337,119 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView defaultGridColor="1" showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="16.3333" defaultRowHeight="19.9" outlineLevelRow="0"/>
   <cols>
-    <col min="1" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col customWidth="1" max="3" min="1" style="1" width="16.3516"/>
+    <col customWidth="1" max="256" min="4" style="1" width="16.3516"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="3">
+    <row customHeight="1" ht="20.25" r="1" s="8">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>transaction_id</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>product_id</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="20.05" r="2" s="8">
+      <c r="A2" s="5" t="n">
+        <v>10001</v>
+      </c>
+      <c r="B2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="C2" s="7" t="n">
+        <v>5.95</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5.355</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="20.05" r="3" s="8">
+      <c r="A3" s="5" t="n">
+        <v>10002</v>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>2</v>
       </c>
+      <c r="C3" s="7" t="n">
+        <v>7.56</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6.803999999999999</v>
+      </c>
     </row>
-    <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" s="5">
-        <v>10001</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7">
-        <v>5.95</v>
+    <row customHeight="1" ht="20.05" r="4" s="8">
+      <c r="A4" s="5" t="n">
+        <v>10003</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3.825</v>
       </c>
     </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="5">
-        <v>10002</v>
-      </c>
-      <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7">
-        <v>7.56</v>
+    <row customHeight="1" ht="20.05" r="5" s="8">
+      <c r="A5" s="5" t="n">
+        <v>10004</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>8.85</v>
+      </c>
+      <c r="D5" t="n">
+        <v>7.965</v>
       </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="5">
-        <v>10003</v>
-      </c>
-      <c r="B4" s="6">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7">
-        <v>4.25</v>
-      </c>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="5">
-        <v>10004</v>
-      </c>
-      <c r="B5" s="6">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7">
-        <v>8.85</v>
-      </c>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="5">
+    <row customHeight="1" ht="20.05" r="6" s="8">
+      <c r="A6" s="5" t="n">
         <v>10005</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="7" t="n">
         <v>2.55</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.295</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins bottom="0.75" footer="0.277778" header="0.277778" left="0.5" right="0.5" top="0.75"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" orientation="portrait" pageOrder="downThenOver" scale="100" useFirstPageNumber="0"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12 &amp;K000000&amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>